<commit_message>
modified EXCEL Acuerdos INE
</commit_message>
<xml_diff>
--- a/src/assets/pdf/AcuerdosINE.xlsx
+++ b/src/assets/pdf/AcuerdosINE.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ATI_02\Documents\sitio-ite\src\assets\pdf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{837FD4B6-9668-4929-A275-F24C6D7999EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91917424-059B-4776-9377-CBF3F9A1B6A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="49860" yWindow="4350" windowWidth="43200" windowHeight="12585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="2020" sheetId="3" r:id="rId1"/>
-    <sheet name="2016" sheetId="2" r:id="rId2"/>
-    <sheet name="2015" sheetId="1" r:id="rId3"/>
+    <sheet name="2022" sheetId="5" r:id="rId1"/>
+    <sheet name="2021" sheetId="4" r:id="rId2"/>
+    <sheet name="2020" sheetId="3" r:id="rId3"/>
+    <sheet name="2016" sheetId="2" r:id="rId4"/>
+    <sheet name="2015" sheetId="1" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="194">
   <si>
     <t>export const dataAcuerdosINE2015 = [</t>
   </si>
@@ -559,6 +561,63 @@
   </si>
   <si>
     <t>ANEXO 2 (PUNTO 4)</t>
+  </si>
+  <si>
+    <t>",link:Acuerdos__pdfpath(`./${"INE/"}${"2021/"}${"</t>
+  </si>
+  <si>
+    <t>export const dataAcuerdosINE2021 = [</t>
+  </si>
+  <si>
+    <t>,year:"2021",numDoc:"INE CG-</t>
+  </si>
+  <si>
+    <t>,year:"2021",numDoc:"INE JGE-</t>
+  </si>
+  <si>
+    <t>2021",nameDoc:"</t>
+  </si>
+  <si>
+    <t>SE APRUEBA EL PLAN INTEGRAL Y LOS CALENDARIOS DE COORDINACIÓN PARA LOS PROCESOS ELECTORALES LOCALES EXTRAORDINARIOS 2021</t>
+  </si>
+  <si>
+    <t>ANEXO 1 PLAN INTEGRAL Y CALENDARIOS DE COORDINACIÓN</t>
+  </si>
+  <si>
+    <t>ANEXO 2 CATÁLOGO DE ACTIVIDADES</t>
+  </si>
+  <si>
+    <t>ANEXO 3 CONCENTRADO DE ACTIVIDADES</t>
+  </si>
+  <si>
+    <t>ACUERDO INCORPORACIÓN TEMPORAL</t>
+  </si>
+  <si>
+    <t>LINEAMIENTOS OPLE INCORPORACIÓN TEMPORAL</t>
+  </si>
+  <si>
+    <t>ACUERDO OCUPACIÓN DE ENCARGOS</t>
+  </si>
+  <si>
+    <t>LINEAMIENTOS OPLE OCUPACIÓN E ENCARGOS</t>
+  </si>
+  <si>
+    <t>ACUERDO POR EL QUE SE APRUEBA LA DESIGNACION DEL CONSEJERO PRESIDENTE PROVISIONAL DEL ITE</t>
+  </si>
+  <si>
+    <t>2022",nameDoc:"</t>
+  </si>
+  <si>
+    <t>",link:Acuerdos__pdfpath(`./${"INE/"}${"2022/"}${"</t>
+  </si>
+  <si>
+    <t>,year:"2022",numDoc:"INE CG-</t>
+  </si>
+  <si>
+    <t>ACUERDO POR EL QUE SE APRUEBA LA DESIGNACIÓN DE LAS PRESIDENCIAS DE LOS OPLES DE LAS ENTIDADES DE AGUASCALIENTES, COAHUILA, NAYARIT, PUEBLA, QUINTANA ROO, SINALOA Y TLAXCALA</t>
+  </si>
+  <si>
+    <t>export const dataAcuerdosINE2022 = [</t>
   </si>
 </sst>
 </file>
@@ -994,11 +1053,421 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6356237-7E3A-475A-B4A7-1C5649528977}">
+  <dimension ref="A2:L5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2:K5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="1.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.140625" customWidth="1"/>
+    <col min="8" max="8" width="46.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="7">
+        <v>1</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="D3" s="15">
+        <v>598</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="I3" s="7">
+        <f>B3</f>
+        <v>1</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3" s="7" t="str">
+        <f t="shared" ref="K3:K4" si="0">CONCATENATE(A3,B3,C3,D3,E3,F3,G3,H3,I3,J3)</f>
+        <v>{id:1,year:"2022",numDoc:"INE CG-598-2022",nameDoc:"ACUERDO POR EL QUE SE APRUEBA LA DESIGNACIÓN DE LAS PRESIDENCIAS DE LOS OPLES DE LAS ENTIDADES DE AGUASCALIENTES, COAHUILA, NAYARIT, PUEBLA, QUINTANA ROO, SINALOA Y TLAXCALA",link:Acuerdos__pdfpath(`./${"INE/"}${"2022/"}${"1.pdf"}`),},</v>
+      </c>
+      <c r="L3" s="7"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="7">
+        <v>2</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="D4" s="15">
+        <v>633</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="I4" s="7">
+        <f>B4</f>
+        <v>2</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>{id:2,year:"2022",numDoc:"INE CG-633-2022",nameDoc:"ACUERDO POR EL QUE SE APRUEBA LA DESIGNACION DEL CONSEJERO PRESIDENTE PROVISIONAL DEL ITE",link:Acuerdos__pdfpath(`./${"INE/"}${"2022/"}${"2.pdf"}`),},</v>
+      </c>
+      <c r="L4" s="7"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC3EF89-481B-4C78-9390-0C3622AE504A}">
+  <dimension ref="A2:L11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K2" sqref="K2:K11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="1.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.140625" customWidth="1"/>
+    <col min="8" max="8" width="46.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="D3" s="3">
+        <v>50</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="I3" s="3">
+        <f>B3</f>
+        <v>1</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K3" s="5"/>
+      <c r="L3" s="7"/>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="I4" s="11" t="str">
+        <f>CONCATENATE(B3,".1")</f>
+        <v>1.1</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="K4" s="13" t="str">
+        <f>CONCATENATE(
+A3,B3,C3,D3,E3,F3,G3,H3,I3,J3,
+A4,B4,C4,D4,E4,F4,G4,H4,I4,J4)</f>
+        <v>{id:1,year:"2021",numDoc:"INE JGE-50-2021",nameDoc:"ACUERDO INCORPORACIÓN TEMPORAL",link:Acuerdos__pdfpath(`./${"INE/"}${"2021/"}${"1.pdf"}`),subRows:[{nameDoc:"LINEAMIENTOS OPLE INCORPORACIÓN TEMPORAL",link:Acuerdos__pdfpath(`./${"INE/"}${"2021/"}${"1.1.pdf"}`),},],},</v>
+      </c>
+      <c r="L4" s="7"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="3">
+        <v>2</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="D5" s="3">
+        <v>51</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="I5" s="3">
+        <f>B5</f>
+        <v>2</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K5" s="5"/>
+      <c r="L5" s="7"/>
+    </row>
+    <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="I6" s="11" t="str">
+        <f>CONCATENATE(B5,".1")</f>
+        <v>2.1</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="K6" s="13" t="str">
+        <f>CONCATENATE(
+A5,B5,C5,D5,E5,F5,G5,H5,I5,J5,
+A6,B6,C6,D6,E6,F6,G6,H6,I6,J6)</f>
+        <v>{id:2,year:"2021",numDoc:"INE JGE-51-2021",nameDoc:"ACUERDO OCUPACIÓN DE ENCARGOS",link:Acuerdos__pdfpath(`./${"INE/"}${"2021/"}${"2.pdf"}`),subRows:[{nameDoc:"LINEAMIENTOS OPLE OCUPACIÓN E ENCARGOS",link:Acuerdos__pdfpath(`./${"INE/"}${"2021/"}${"2.1.pdf"}`),},],},</v>
+      </c>
+      <c r="L6" s="7"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="3">
+        <v>3</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1600</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="I7" s="3">
+        <f>B7</f>
+        <v>3</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K7" s="5"/>
+      <c r="L7" s="7"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="I8" s="7" t="str">
+        <f>CONCATENATE(B7,".1")</f>
+        <v>3.1</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="K8" s="9"/>
+      <c r="L8" s="7"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="I9" s="7" t="str">
+        <f>CONCATENATE(B7,".2")</f>
+        <v>3.2</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="K9" s="9"/>
+      <c r="L9" s="7"/>
+    </row>
+    <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="I10" s="11" t="str">
+        <f>CONCATENATE(B7,".3")</f>
+        <v>3.3</v>
+      </c>
+      <c r="J10" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="K10" s="13" t="str">
+        <f>CONCATENATE(
+A7,B7,C7,D7,E7,F7,G7,H7,I7,J7,
+A8,B8,C8,D8,E8,F8,G8,H8,I8,J8,
+A10,B10,C10,D10,E10,F10,G10,H10,I10,J10)</f>
+        <v>{id:3,year:"2021",numDoc:"INE CG-1600-2021",nameDoc:"SE APRUEBA EL PLAN INTEGRAL Y LOS CALENDARIOS DE COORDINACIÓN PARA LOS PROCESOS ELECTORALES LOCALES EXTRAORDINARIOS 2021",link:Acuerdos__pdfpath(`./${"INE/"}${"2021/"}${"3.pdf"}`),subRows:[{nameDoc:"ANEXO 1 PLAN INTEGRAL Y CALENDARIOS DE COORDINACIÓN",link:Acuerdos__pdfpath(`./${"INE/"}${"2021/"}${"3.1.pdf"}`),},{nameDoc:"ANEXO 3 CONCENTRADO DE ACTIVIDADES",link:Acuerdos__pdfpath(`./${"INE/"}${"2021/"}${"3.3.pdf"}`),},],},</v>
+      </c>
+      <c r="L10" s="7"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC0BB564-5A1A-4E73-95B4-61D8F647798A}">
   <dimension ref="A2:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:K16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1479,7 +1948,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D8B093F-CDAF-451A-BD9D-C47671DFE6FB}">
   <dimension ref="A2:N29"/>
   <sheetViews>
@@ -2441,7 +2910,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:O70"/>
   <sheetViews>

</xml_diff>